<commit_message>
Year to Year form bug fixes
</commit_message>
<xml_diff>
--- a/Year to Year.xlsx
+++ b/Year to Year.xlsx
@@ -170,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -186,8 +186,11 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="10" xfId="0" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="10" xfId="0" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
@@ -257,401 +260,401 @@
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="str">
-        <f>SUM((-B2+D2)/B2)</f>
+        <f t="shared" ref="C2:C13" si="1">SUM((-B2+D2)/B2)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="str">
-        <f>SUM((-D2+F2)/D2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F2" s="5"/>
+        <f t="shared" ref="E2:E13" si="2">SUM((-D2+F2)/D2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F2" s="7"/>
       <c r="G2" s="6" t="str">
-        <f>SUM((-F2+H2)/F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H2" s="5"/>
+        <f t="shared" ref="G2:G13" si="3">SUM((-F2+H2)/F2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H2" s="7"/>
       <c r="I2" s="6" t="str">
-        <f>SUM((-H2+J2)/H2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J2" s="5"/>
+        <f t="shared" ref="I2:I13" si="4">SUM((-H2+J2)/H2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="str">
-        <f>SUM((-B2+D2)/B2)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6" t="str">
-        <f>SUM((-D2+F2)/D2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F3" s="5"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F3" s="7"/>
       <c r="G3" s="6" t="str">
-        <f>SUM((-F2+H2)/F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H3" s="5"/>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H3" s="7"/>
       <c r="I3" s="6" t="str">
-        <f>SUM((-H2+J2)/H2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J3" s="5"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="6" t="str">
-        <f>SUM((-B2+D2)/B2)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6" t="str">
-        <f>SUM((-D2+F2)/D2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F4" s="5"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F4" s="7"/>
       <c r="G4" s="6" t="str">
-        <f>SUM((-F2+H2)/F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H4" s="5"/>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H4" s="7"/>
       <c r="I4" s="6" t="str">
-        <f>SUM((-H2+J2)/H2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J4" s="5"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="str">
-        <f>SUM((-B2+D2)/B2)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6" t="str">
-        <f>SUM((-D2+F2)/D2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F5" s="5"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F5" s="7"/>
       <c r="G5" s="6" t="str">
-        <f>SUM((-F2+H2)/F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H5" s="5"/>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" s="7"/>
       <c r="I5" s="6" t="str">
-        <f>SUM((-H2+J2)/H2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J5" s="5"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6" t="str">
-        <f>SUM((-B2+D2)/B2)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6" t="str">
-        <f>SUM((-D2+F2)/D2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" s="5"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F6" s="7"/>
       <c r="G6" s="6" t="str">
-        <f>SUM((-F2+H2)/F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H6" s="5"/>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H6" s="7"/>
       <c r="I6" s="6" t="str">
-        <f>SUM((-H2+J2)/H2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J6" s="5"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6" t="str">
-        <f>SUM((-B2+D2)/B2)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="str">
-        <f>SUM((-D2+F2)/D2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F7" s="5"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F7" s="7"/>
       <c r="G7" s="6" t="str">
-        <f>SUM((-F2+H2)/F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" s="5"/>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" s="7"/>
       <c r="I7" s="6" t="str">
-        <f>SUM((-H2+J2)/H2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J7" s="5"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="6" t="str">
-        <f>SUM((-B2+D2)/B2)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="str">
-        <f>SUM((-D2+F2)/D2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F8" s="5"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F8" s="7"/>
       <c r="G8" s="6" t="str">
-        <f>SUM((-F2+H2)/F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="5"/>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" s="7"/>
       <c r="I8" s="6" t="str">
-        <f>SUM((-H2+J2)/H2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J8" s="5"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J8" s="7"/>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="str">
-        <f>SUM((-B2+D2)/B2)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6" t="str">
-        <f>SUM((-D2+F2)/D2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F9" s="5"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F9" s="7"/>
       <c r="G9" s="6" t="str">
-        <f>SUM((-F2+H2)/F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9" s="5"/>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H9" s="7"/>
       <c r="I9" s="6" t="str">
-        <f>SUM((-H2+J2)/H2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J9" s="5"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9" s="7"/>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="6" t="str">
-        <f>SUM((-B2+D2)/B2)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="str">
-        <f>SUM((-D2+F2)/D2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" s="5"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F10" s="7"/>
       <c r="G10" s="6" t="str">
-        <f>SUM((-F2+H2)/F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H10" s="5"/>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" s="7"/>
       <c r="I10" s="6" t="str">
-        <f>SUM((-H2+J2)/H2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J10" s="5"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" s="7"/>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="6" t="str">
-        <f>SUM((-B2+D2)/B2)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="6" t="str">
-        <f>SUM((-D2+F2)/D2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" s="5"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" s="7"/>
       <c r="G11" s="6" t="str">
-        <f>SUM((-F2+H2)/F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H11" s="5"/>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" s="7"/>
       <c r="I11" s="6" t="str">
-        <f>SUM((-H2+J2)/H2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J11" s="5"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" s="7"/>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="6" t="str">
-        <f>SUM((-B2+D2)/B2)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="6" t="str">
-        <f>SUM((-D2+F2)/D2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F12" s="5"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F12" s="7"/>
       <c r="G12" s="6" t="str">
-        <f>SUM((-F2+H2)/F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H12" s="5"/>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H12" s="7"/>
       <c r="I12" s="6" t="str">
-        <f>SUM((-H2+J2)/H2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J12" s="5"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12" s="7"/>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="6" t="str">
-        <f>SUM((-B2+D2)/B2)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="6" t="str">
-        <f>SUM((-D2+F2)/D2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="5"/>
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" s="7"/>
       <c r="G13" s="6" t="str">
-        <f>SUM((-F2+H2)/F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H13" s="5"/>
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H13" s="7"/>
       <c r="I13" s="6" t="str">
-        <f>SUM((-H2+J2)/H2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J13" s="5"/>
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" s="7"/>
     </row>
     <row r="14">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="13">
         <f>SUM(B2:B13)</f>
         <v>0</v>
       </c>
       <c r="C15" s="6" t="str">
-        <f t="shared" ref="C15:C16" si="1">SUM((-B4+D4)/B4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D15" s="12">
+        <f t="shared" ref="C15:C16" si="5">SUM((-B15+D15)/B15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D15" s="13">
         <f>SUM(D2:D13)</f>
         <v>0</v>
       </c>
       <c r="E15" s="6" t="str">
-        <f t="shared" ref="E15:E16" si="2">SUM((-D4+F4)/D4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F15" s="12">
+        <f t="shared" ref="E15:E16" si="6">SUM((-D15+F15)/D15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" s="13">
         <f>SUM(F2:F13)</f>
         <v>0</v>
       </c>
       <c r="G15" s="6" t="str">
-        <f t="shared" ref="G15:G16" si="3">SUM((-F4+H4)/F4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="12">
+        <f t="shared" ref="G15:G16" si="7">SUM((-F15+H15)/F15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="13">
         <f>SUM(H2:H13)</f>
         <v>0</v>
       </c>
       <c r="I15" s="6" t="str">
-        <f t="shared" ref="I15:I16" si="4">SUM((-H4+J4)/H4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J15" s="12">
+        <f t="shared" ref="I15:I16" si="8">SUM((-H15+J15)/H15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="13">
         <f>SUM(J2:J13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="13">
         <f>(B15/12)</f>
         <v>0</v>
       </c>
       <c r="C16" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D16" s="12">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D16" s="13">
         <f>(D15/12)</f>
         <v>0</v>
       </c>
       <c r="E16" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F16" s="12">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" s="13">
         <f>(F15/12)</f>
         <v>0</v>
       </c>
       <c r="G16" s="6" t="str">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H16" s="12">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="13">
         <f>(H15/12)</f>
         <v>0</v>
       </c>
       <c r="I16" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J16" s="12">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" s="13">
         <f>(J15/12)</f>
         <v>0</v>
       </c>

</xml_diff>